<commit_message>
updated Planning 4.4 - 11.4
</commit_message>
<xml_diff>
--- a/Planning/Planning_4_4_11_4.xlsx
+++ b/Planning/Planning_4_4_11_4.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B378416-158D-434F-8ED4-20A21A12BE42}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143BA97B-3D16-4C6C-ADAB-0EC4866F97B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -76,16 +76,13 @@
     <t>Trinkl, Punz, Strutzenberger</t>
   </si>
   <si>
-    <t>5h</t>
-  </si>
-  <si>
     <t>6h</t>
   </si>
   <si>
     <t>4h</t>
   </si>
   <si>
-    <t>1h</t>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -443,13 +440,13 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -463,13 +460,13 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
@@ -511,13 +508,13 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>

</xml_diff>